<commit_message>
I finished to created a new NER model based on HarryPotter and trained it for 30 Epochs
</commit_message>
<xml_diff>
--- a/23-guardias-agd-nlp/Solucion.xlsx
+++ b/23-guardias-agd-nlp/Solucion.xlsx
@@ -1,65 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emarcelloni\Documents\machine-learning\23-guardias-agd-nlp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Solución</t>
-  </si>
-  <si>
-    <t>Me comunico con Nico Jacob quien me indica que puede estar caída la replica de Alejandro Roca. Me comunico con la Guardia DBA quien confirma que la replica esta caída y junto con Martin Alfonso solucionan el problema. Llamo nuevamente a PAG y les indico que todo esta funcionando correctamente y que cualquier novedad nos tengan al tanto.</t>
-  </si>
-  <si>
-    <t>Me contacto con Nicolas Jacob, le explico la situación y me indica que le pida al usuario que baje los camiones de las balanza y reinicien el sistema. Me comunico con el usuario le traslado lo comentado y le indico que si seguía con el inconveniente posterior al reinicio que me llame nuevamente.</t>
-  </si>
-  <si>
-    <t>Se indica que es un problema operativo que debe resolver con su supervisor o soporte playa.</t>
-  </si>
-  <si>
-    <t>Se consulta que los pesos y efectivamente estan correctos. Se llama a la guardia de DBA para consultar si hay alguna replica bloqueda desde Alejandro hacia el central. Gaston Mignola revisa y corrobora que hay un problema. Luego de levantar la replica se le informa al usuario que indica que pudo pesar con normalidad</t>
-  </si>
-  <si>
-    <t>Se derivó a Soporte Playa por tener resolución operativa</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -74,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -398,61 +420,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1139</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>581</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Problema</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Solución</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>En Beltran les da error ORA-CLi al confirmar arribo ctg en afip</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Se le explica que es un error de los servidores de afip. No podemos hacer nada al respecto.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>En su notebook no puede ver los iconos de acceso al sistema de playa.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Me comunico con F Garay para explicarle el problema y me indica que lo debe ver juan ochoa para verificar que este bien el perfil del usuario.
+Se deriva a la guardia secundaria.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>785</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>En carga de vagones el sistema no tomaba todos los dígitos del peso</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Se cambio la configuración en msbal.ini</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Error en Playa al momento de Tomar Muestra en Boquilleo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>El usuario informa un problema/error en el sistema de playa al momento de generar una muestra de boquilleo el cual le indica una error de COBOL paraciera como que falta un DLL, me comunico con la guardia de Sistema Playa en el cual Mauro Calavgni me comento que van a seguir el caso.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guardia Principal me deriva el caso: En acopio Beltran tiene problema con la balanza, En el romaneo falta el dato de humedad. </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Me comunico con el usuario quien me indica que ya lo habian resuelto operativamente.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>599</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>No pasa dato de playa a sistema de acopios</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acopio María Teresa - Javier (guardia DBA), indica que el problema es debido a una carta de porte duplicada (utilizada en 2 plantas). Se constata con el usuario Paola Rippol. Se comunica a soporte playa (Germán Recosta), toma el caso para que lo solucionen por vías operativas. Luego Germán solicita se borren el dato duplicado. Guardia DBA borra el dato correspondiente. Se toma contacto con el usuario y se valida la solución del problema. </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Desde carga de datos de UNCO no pueden acceder al servidor de Timbues</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Se deriva a guardia de tecnologia</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>En acopio Bouchardo no pueden ingresar al sistema de Playa. Error SQL -1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Se contacta a guardia dba para que levante el servicio SQL luego se contacta al usuario para que verifique la solucion</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>956</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">En el Sistema de Producción, el usuario no veía los turnos.  </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Se encontraba caída la réplica de Central a PMA. Se llamo a guardia DBA. Pablo Centeno destrabó la replica.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>En la PC de entregadores1 le da error 93 al exportar a excel desde Playa</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Se toma asistencia, se verifican los permisos de usuario sobre la carpeta. Al estar bien se solicita que reinicie la sesión para renovar credenciales. Se soluciona el problema.</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>